<commit_message>
Cleaned up files and code
</commit_message>
<xml_diff>
--- a/Escherichia_coli_REL606/conditions_data.xlsx
+++ b/Escherichia_coli_REL606/conditions_data.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="660" windowWidth="20595" windowHeight="10425"/>
+    <workbookView xWindow="600" yWindow="720" windowWidth="20595" windowHeight="10365"/>
   </bookViews>
   <sheets>
     <sheet name="41598_2017_BFsrep45303_MOESM52_" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1789,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="I137" sqref="I137"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14022,7 +14022,7 @@
   <dimension ref="A1:FP2"/>
   <sheetViews>
     <sheetView topLeftCell="EW1" workbookViewId="0">
-      <selection activeCell="FE8" sqref="FE8"/>
+      <selection activeCell="Q1" sqref="Q1:FP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>